<commit_message>
Test Data with fixed start
</commit_message>
<xml_diff>
--- a/3D analysis/Data_1_joint/40deg/Test40deg - Lentgh.xlsx
+++ b/3D analysis/Data_1_joint/40deg/Test40deg - Lentgh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anselme\Documents\GitHub\soft_robot_manipulator\3D analysis\Data_1_joint\40deg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD313A2-3BDC-4D0B-B26D-25263C3E0D27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A5BBE0-A978-443A-AE40-8B5BCC045D29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
-    <pivotCache cacheId="12" r:id="rId8"/>
+    <pivotCache cacheId="6" r:id="rId7"/>
+    <pivotCache cacheId="7" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -32111,7 +32111,193 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6E55786B-2E11-4695-A46A-29A366A7613C}" name="Tableau croisé dynamique3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6C76F14C-FAF9-49A9-9796-A3E08F0EB2E9}" name="Tableau croisé dynamique14" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="T31:AY34" firstHeaderRow="1" firstDataRow="3" firstDataCol="0"/>
+  <pivotFields count="11">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="31">
+        <item m="1" x="23"/>
+        <item m="1" x="21"/>
+        <item m="1" x="19"/>
+        <item m="1" x="17"/>
+        <item m="1" x="15"/>
+        <item m="1" x="29"/>
+        <item m="1" x="28"/>
+        <item m="1" x="27"/>
+        <item m="1" x="26"/>
+        <item m="1" x="25"/>
+        <item m="1" x="24"/>
+        <item m="1" x="22"/>
+        <item m="1" x="20"/>
+        <item m="1" x="18"/>
+        <item m="1" x="16"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="2">
+    <field x="2"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="32">
+    <i>
+      <x v="15"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="16"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="17"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="18"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="19"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="20"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="21"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="22"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="23"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="24"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="25"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="26"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="27"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="28"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="29"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Moyenne de longueur cm" fld="8" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Écartype de longueur cm" fld="8" subtotal="stdDev" baseField="1" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6E55786B-2E11-4695-A46A-29A366A7613C}" name="Tableau croisé dynamique3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="T5:Y25" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0">
@@ -32571,194 +32757,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6C76F14C-FAF9-49A9-9796-A3E08F0EB2E9}" name="Tableau croisé dynamique14" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="T31:AY34" firstHeaderRow="1" firstDataRow="3" firstDataCol="0"/>
-  <pivotFields count="11">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="31">
-        <item m="1" x="23"/>
-        <item m="1" x="21"/>
-        <item m="1" x="19"/>
-        <item m="1" x="17"/>
-        <item m="1" x="15"/>
-        <item m="1" x="29"/>
-        <item m="1" x="28"/>
-        <item m="1" x="27"/>
-        <item m="1" x="26"/>
-        <item m="1" x="25"/>
-        <item m="1" x="24"/>
-        <item m="1" x="22"/>
-        <item m="1" x="20"/>
-        <item m="1" x="18"/>
-        <item m="1" x="16"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colFields count="2">
-    <field x="2"/>
-    <field x="-2"/>
-  </colFields>
-  <colItems count="32">
-    <i>
-      <x v="15"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="16"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="17"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="18"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="19"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="20"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="21"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="22"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="23"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="24"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="25"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="26"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="27"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="28"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="29"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Moyenne de longueur cm" fld="8" subtotal="average" baseField="1" baseItem="0"/>
-    <dataField name="Écartype de longueur cm" fld="8" subtotal="stdDev" baseField="1" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C3621364-8EFD-47D8-A75D-947829DEA369}" name="Tableau croisé dynamique15" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C3621364-8EFD-47D8-A75D-947829DEA369}" name="Tableau croisé dynamique15" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:AF6" firstHeaderRow="1" firstDataRow="3" firstDataCol="0"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -32944,7 +32944,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6810F8AC-CE6B-4B49-B6FF-0C89630B1001}" name="Tableau croisé dynamique15" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6810F8AC-CE6B-4B49-B6FF-0C89630B1001}" name="Tableau croisé dynamique15" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:AF6" firstHeaderRow="1" firstDataRow="3" firstDataCol="0"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -33130,7 +33130,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{056A63FF-B9D0-4081-A3F5-2B29DA6C2F87}" name="Tableau croisé dynamique15" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{056A63FF-B9D0-4081-A3F5-2B29DA6C2F87}" name="Tableau croisé dynamique15" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:AF6" firstHeaderRow="1" firstDataRow="3" firstDataCol="0" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -34073,7 +34073,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3880E5FA-4226-4020-9DD3-3F50F0E253DB}" name="Tableau croisé dynamique15" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3880E5FA-4226-4020-9DD3-3F50F0E253DB}" name="Tableau croisé dynamique15" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:AF6" firstHeaderRow="1" firstDataRow="3" firstDataCol="0"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -34259,7 +34259,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4F23CF0F-D60F-4A17-9798-9A2D4AB34A64}" name="Tableau croisé dynamique15" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4F23CF0F-D60F-4A17-9798-9A2D4AB34A64}" name="Tableau croisé dynamique15" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:AF6" firstHeaderRow="1" firstDataRow="3" firstDataCol="0"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -34743,7 +34743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:TR451"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G303" sqref="G303"/>
     </sheetView>
   </sheetViews>
@@ -54462,7 +54462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8E32B1-490F-49BF-8ADA-57F525EBB13E}">
   <dimension ref="A1:AF10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -54933,7 +54933,7 @@
   <dimension ref="A3:AF10"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>